<commit_message>
update timesheet period may to june
</commit_message>
<xml_diff>
--- a/6_Period_20_May_2024_sd_19_Jun_2024/Timesheet Danamon-Bayu Bagus Bagaswara-Mei.xlsx
+++ b/6_Period_20_May_2024_sd_19_Jun_2024/Timesheet Danamon-Bayu Bagus Bagaswara-Mei.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\timesheet-danamon\6_Period_20_May_2024_sd_19_Jun_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\6_Period_20_May_2024_sd_19_Jun_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692A9FF2-D544-45CE-A0A1-8AE5F75654D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF7ABE0-E454-4130-9079-12EE9E1FB3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,16 +175,16 @@
     <t>Bayu Bagus Bagaswara</t>
   </si>
   <si>
-    <t>Diskusi alur bisnis Billing dengan User</t>
-  </si>
-  <si>
-    <t>Pengembangan fitur Billing</t>
-  </si>
-  <si>
     <t>Diskusi dengan tim developer Billing</t>
   </si>
   <si>
-    <t>20 Mei - 19 Juni</t>
+    <t>Support SIT Release 8 (Billing)</t>
+  </si>
+  <si>
+    <t>Support  UAT Release 8 (Billing)</t>
+  </si>
+  <si>
+    <t>20 May - 19 June</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,9 +646,6 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1107,8 +1104,8 @@
   </sheetPr>
   <dimension ref="A1:EQ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH13" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
@@ -1205,10 +1202,10 @@
       </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-      <c r="S5" s="71" t="s">
+      <c r="S5" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="72"/>
+      <c r="T5" s="71"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10" t="s">
         <v>24</v>
@@ -1235,47 +1232,47 @@
       <c r="B6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="73" t="s">
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="75"/>
-      <c r="S6" s="76">
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="75">
         <v>2024</v>
       </c>
-      <c r="T6" s="77"/>
-      <c r="U6" s="76" t="s">
+      <c r="T6" s="76"/>
+      <c r="U6" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
-      <c r="X6" s="70"/>
-      <c r="Y6" s="70"/>
-      <c r="Z6" s="77"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="76"/>
       <c r="AA6" s="23"/>
-      <c r="AB6" s="70"/>
-      <c r="AC6" s="70"/>
-      <c r="AD6" s="70"/>
-      <c r="AE6" s="70"/>
-      <c r="AF6" s="60"/>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="59"/>
-      <c r="AI6" s="59"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69"/>
+      <c r="AF6" s="59"/>
+      <c r="AG6" s="57"/>
+      <c r="AH6" s="58"/>
+      <c r="AI6" s="58"/>
       <c r="AJ6" s="24"/>
     </row>
     <row r="7" spans="1:147" s="1" customFormat="1" ht="15" customHeight="1">
@@ -1540,10 +1537,10 @@
       <c r="E10" s="49">
         <v>1</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
       <c r="J10" s="49">
         <v>1</v>
       </c>
@@ -1559,8 +1556,8 @@
       <c r="N10" s="49">
         <v>1</v>
       </c>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
       <c r="Q10" s="49">
         <v>1</v>
       </c>
@@ -1576,8 +1573,8 @@
       <c r="U10" s="49">
         <v>1</v>
       </c>
-      <c r="V10" s="55"/>
-      <c r="W10" s="55"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
       <c r="X10" s="49">
         <v>1</v>
       </c>
@@ -1593,10 +1590,10 @@
       <c r="AB10" s="49">
         <v>1</v>
       </c>
-      <c r="AC10" s="55"/>
-      <c r="AD10" s="56"/>
-      <c r="AE10" s="62"/>
-      <c r="AF10" s="62"/>
+      <c r="AC10" s="54"/>
+      <c r="AD10" s="55"/>
+      <c r="AE10" s="61"/>
+      <c r="AF10" s="61"/>
       <c r="AG10" s="50">
         <v>1</v>
       </c>
@@ -1604,10 +1601,10 @@
         <f>SUM(C10:AG10)</f>
         <v>19</v>
       </c>
-      <c r="AI10" s="64" t="s">
+      <c r="AI10" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="AJ10" s="66"/>
+      <c r="AJ10" s="65"/>
       <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
       <c r="AM10" s="6"/>
@@ -1723,141 +1720,217 @@
     <row r="11" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A11" s="36"/>
       <c r="B11" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="50"/>
-      <c r="U11" s="50"/>
-      <c r="V11" s="56"/>
-      <c r="W11" s="56"/>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="50"/>
-      <c r="Z11" s="50"/>
+        <v>27</v>
+      </c>
+      <c r="C11" s="50">
+        <v>1</v>
+      </c>
+      <c r="D11" s="50">
+        <v>1</v>
+      </c>
+      <c r="E11" s="52">
+        <v>1</v>
+      </c>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="50">
+        <v>1</v>
+      </c>
+      <c r="K11" s="50">
+        <v>1</v>
+      </c>
+      <c r="L11" s="50">
+        <v>1</v>
+      </c>
+      <c r="M11" s="50">
+        <v>1</v>
+      </c>
+      <c r="N11" s="50">
+        <v>1</v>
+      </c>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="50">
+        <v>1</v>
+      </c>
+      <c r="R11" s="50">
+        <v>1</v>
+      </c>
+      <c r="S11" s="44">
+        <v>1</v>
+      </c>
+      <c r="T11" s="50">
+        <v>1</v>
+      </c>
+      <c r="U11" s="50">
+        <v>1</v>
+      </c>
+      <c r="V11" s="55"/>
+      <c r="W11" s="55"/>
+      <c r="X11" s="50">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="50">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="50">
+        <v>1</v>
+      </c>
       <c r="AA11" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB11" s="50">
-        <v>2</v>
-      </c>
-      <c r="AC11" s="56"/>
-      <c r="AD11" s="56"/>
-      <c r="AE11" s="62"/>
-      <c r="AF11" s="62"/>
-      <c r="AG11" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="AC11" s="55"/>
+      <c r="AD11" s="55"/>
+      <c r="AE11" s="61"/>
+      <c r="AF11" s="61"/>
+      <c r="AG11" s="50">
+        <v>1</v>
+      </c>
       <c r="AH11" s="44">
         <f>SUM(C11:AG11)</f>
-        <v>4</v>
-      </c>
-      <c r="AI11" s="65"/>
-      <c r="AJ11" s="67"/>
+        <v>19</v>
+      </c>
+      <c r="AI11" s="64"/>
+      <c r="AJ11" s="66"/>
     </row>
     <row r="12" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A12" s="36"/>
       <c r="B12" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="56"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="56"/>
-      <c r="W12" s="56"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="50"/>
-      <c r="Z12" s="50"/>
-      <c r="AA12" s="50"/>
-      <c r="AB12" s="50"/>
-      <c r="AC12" s="56"/>
-      <c r="AD12" s="56"/>
-      <c r="AE12" s="62"/>
-      <c r="AF12" s="62"/>
+        <v>28</v>
+      </c>
+      <c r="C12" s="50">
+        <v>6</v>
+      </c>
+      <c r="D12" s="50">
+        <v>6</v>
+      </c>
+      <c r="E12" s="52">
+        <v>6</v>
+      </c>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="50">
+        <v>6</v>
+      </c>
+      <c r="K12" s="50">
+        <v>6</v>
+      </c>
+      <c r="L12" s="50">
+        <v>6</v>
+      </c>
+      <c r="M12" s="50">
+        <v>6</v>
+      </c>
+      <c r="N12" s="50">
+        <v>6</v>
+      </c>
+      <c r="O12" s="55"/>
+      <c r="P12" s="55"/>
+      <c r="Q12" s="50">
+        <v>6</v>
+      </c>
+      <c r="R12" s="50">
+        <v>6</v>
+      </c>
+      <c r="S12" s="44">
+        <v>6</v>
+      </c>
+      <c r="T12" s="50">
+        <v>6</v>
+      </c>
+      <c r="U12" s="50">
+        <v>6</v>
+      </c>
+      <c r="V12" s="55"/>
+      <c r="W12" s="55"/>
+      <c r="X12" s="50">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="50">
+        <v>5</v>
+      </c>
+      <c r="Z12" s="50">
+        <v>5</v>
+      </c>
+      <c r="AA12" s="50">
+        <v>5</v>
+      </c>
+      <c r="AB12" s="50">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="55"/>
+      <c r="AD12" s="55"/>
+      <c r="AE12" s="61"/>
+      <c r="AF12" s="61"/>
       <c r="AG12" s="50"/>
       <c r="AH12" s="44">
         <f>SUM(C12:AG12)</f>
-        <v>0</v>
-      </c>
-      <c r="AI12" s="65"/>
-      <c r="AJ12" s="67"/>
+        <v>103</v>
+      </c>
+      <c r="AI12" s="64"/>
+      <c r="AJ12" s="66"/>
     </row>
     <row r="13" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A13" s="36"/>
       <c r="B13" s="47" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
       <c r="E13" s="52"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
       <c r="L13" s="50"/>
       <c r="M13" s="50"/>
       <c r="N13" s="50"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
       <c r="Q13" s="50"/>
       <c r="R13" s="50"/>
       <c r="S13" s="44"/>
       <c r="T13" s="50"/>
       <c r="U13" s="50"/>
-      <c r="V13" s="56"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="50"/>
+      <c r="V13" s="55"/>
+      <c r="W13" s="55"/>
+      <c r="X13" s="50">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="50">
+        <v>1</v>
+      </c>
       <c r="Z13" s="50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA13" s="50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB13" s="50">
-        <v>5</v>
-      </c>
-      <c r="AC13" s="56"/>
-      <c r="AD13" s="56"/>
-      <c r="AE13" s="62"/>
-      <c r="AF13" s="62"/>
-      <c r="AG13" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="AC13" s="55"/>
+      <c r="AD13" s="55"/>
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="61"/>
+      <c r="AG13" s="50">
+        <v>6</v>
+      </c>
       <c r="AH13" s="44">
         <f>SUM(C13:AG13)</f>
-        <v>15</v>
-      </c>
-      <c r="AI13" s="65"/>
-      <c r="AJ13" s="67"/>
+        <v>11</v>
+      </c>
+      <c r="AI13" s="64"/>
+      <c r="AJ13" s="66"/>
     </row>
     <row r="14" spans="1:147" s="4" customFormat="1" ht="36" customHeight="1">
       <c r="A14" s="37" t="s">
@@ -1866,93 +1939,93 @@
       <c r="B14" s="38"/>
       <c r="C14" s="51">
         <f t="shared" ref="C14:AG14" si="0">SUM(C10:C13)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F14" s="63">
+        <v>8</v>
+      </c>
+      <c r="F14" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="63">
+      <c r="G14" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="57">
+      <c r="H14" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I14" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="N14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
+        <v>8</v>
+      </c>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
       <c r="Q14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="R14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="S14" s="45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="T14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="U14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V14" s="57">
+        <v>8</v>
+      </c>
+      <c r="V14" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W14" s="57">
+      <c r="W14" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Y14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Z14" s="51">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AA14" s="51">
         <f t="shared" si="0"/>
@@ -1962,29 +2035,29 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="AC14" s="57">
+      <c r="AC14" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD14" s="57">
+      <c r="AD14" s="56">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE14" s="63">
+      <c r="AE14" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF14" s="63">
+      <c r="AF14" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AH14" s="45">
         <f>SUM(C14:AG14)</f>
-        <v>38</v>
+        <v>152</v>
       </c>
       <c r="AI14" s="39"/>
       <c r="AJ14" s="40"/>

</xml_diff>